<commit_message>
added other BERT example
</commit_message>
<xml_diff>
--- a/data/annotations/indicators_and_annotations-v7.xlsx
+++ b/data/annotations/indicators_and_annotations-v7.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreaballatore/Dropbox/DRBX_Docs/Work/Projects/github_projects/museums-in-the-pandemic/data/annotations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEBBD1BD-EC33-9845-A49E-724A57F773B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06DC2F70-3089-104A-91B7-0F566A3B86FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="22620" windowHeight="21100" activeTab="1" xr2:uid="{B946F43B-58A6-4248-B453-C61D9D19EABF}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="22620" windowHeight="16520" activeTab="1" xr2:uid="{B946F43B-58A6-4248-B453-C61D9D19EABF}"/>
   </bookViews>
   <sheets>
     <sheet name="indicators" sheetId="3" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1666" uniqueCount="789">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1667" uniqueCount="789">
   <si>
     <t>indicator_code</t>
   </si>
@@ -3546,8 +3546,8 @@
   <dimension ref="A1:I279"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="143" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A207" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F216" sqref="F216"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6721,6 +6721,9 @@
       </c>
       <c r="E215" s="5" t="s">
         <v>267</v>
+      </c>
+      <c r="F215" s="5" t="s">
+        <v>772</v>
       </c>
     </row>
     <row r="216" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -10222,21 +10225,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002C2CD1DD118472458A0E6161F2144773" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d6e70606a31341017029f9eff1eb720b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0afe7543-80e5-4676-a63d-5a4feeb00470" xmlns:ns3="0accda53-abec-4882-afe9-cc0ba02332f1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b75b586682df3983c7d47b6a8e259e8b" ns2:_="" ns3:_="">
     <xsd:import namespace="0afe7543-80e5-4676-a63d-5a4feeb00470"/>
@@ -10447,24 +10435,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73852CBC-2E2A-43EB-ADAD-FD0ACC658E1E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CD2911FF-F89D-4904-8999-6B7B74F09443}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70C858A0-B59C-47E8-A200-4A6AAC57C6A6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10481,4 +10467,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CD2911FF-F89D-4904-8999-6B7B74F09443}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73852CBC-2E2A-43EB-ADAD-FD0ACC658E1E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>